<commit_message>
upload new evidence map
</commit_message>
<xml_diff>
--- a/raw-data/RSV_attribute_hierarchy_Dec.xlsx
+++ b/raw-data/RSV_attribute_hierarchy_Dec.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deborah/Library/CloudStorage/GoogleDrive-deborahcromer@gmail.com/Other computers/Work Blue Computer/github/RSVcorrelates/raw-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/z2211982/github/RSVcorrelates/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BA507A-8BF0-3E4C-8D8F-C7C9FD2ABB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A23468B-9509-A346-8D83-D564AFB30B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6700" yWindow="1340" windowWidth="39280" windowHeight="20860" xr2:uid="{E5577812-52DB-7549-9224-56C8E4FDF043}"/>
+    <workbookView xWindow="5520" yWindow="1340" windowWidth="39280" windowHeight="20860" xr2:uid="{E5577812-52DB-7549-9224-56C8E4FDF043}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="84">
   <si>
     <t>level_1_attribute</t>
   </si>
@@ -164,18 +164,12 @@
     <t>Not Approved</t>
   </si>
   <si>
-    <t>Approval Unclassified</t>
-  </si>
-  <si>
     <t>approved</t>
   </si>
   <si>
     <t>not approved</t>
   </si>
   <si>
-    <t>approval unknown</t>
-  </si>
-  <si>
     <t>combination vaccine:not approved</t>
   </si>
   <si>
@@ -203,9 +197,6 @@
     <t>virus-like particles:not approved</t>
   </si>
   <si>
-    <t>Approval Status (simple)</t>
-  </si>
-  <si>
     <t>Product and Approval Details</t>
   </si>
   <si>
@@ -246,6 +237,60 @@
   </si>
   <si>
     <t>2_maternal_passive_immunogenicity</t>
+  </si>
+  <si>
+    <t>mRNA:not approved</t>
+  </si>
+  <si>
+    <t>formalin inactivated:not approved</t>
+  </si>
+  <si>
+    <t>Formalin Inactivated Vaccine</t>
+  </si>
+  <si>
+    <t>Product Details</t>
+  </si>
+  <si>
+    <t>monoclonal antibody</t>
+  </si>
+  <si>
+    <t>protein subunit</t>
+  </si>
+  <si>
+    <t>mRNA</t>
+  </si>
+  <si>
+    <t>live-attenuated</t>
+  </si>
+  <si>
+    <t>viral vector</t>
+  </si>
+  <si>
+    <t>virus-like particles</t>
+  </si>
+  <si>
+    <t>combination vaccine</t>
+  </si>
+  <si>
+    <t>formalin inactivated</t>
+  </si>
+  <si>
+    <t>Approval Status</t>
+  </si>
+  <si>
+    <t>Population Tested</t>
+  </si>
+  <si>
+    <t>infants_children</t>
+  </si>
+  <si>
+    <t>maternal</t>
+  </si>
+  <si>
+    <t>general_adults</t>
+  </si>
+  <si>
+    <t>older_adults</t>
   </si>
 </sst>
 </file>
@@ -267,7 +312,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,6 +337,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -305,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -329,6 +392,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B74C7C1-39D6-4543-AF62-37F03D7DCD25}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -726,10 +807,10 @@
         <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -740,10 +821,10 @@
         <v>7</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -768,10 +849,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -782,10 +863,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -810,10 +891,10 @@
         <v>10</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -824,10 +905,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -852,10 +933,10 @@
         <v>8</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -866,10 +947,10 @@
         <v>8</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -953,61 +1034,66 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="A22" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="C22" s="15"/>
+      <c r="D22" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" t="s">
-        <v>44</v>
+      <c r="A24" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>48</v>
@@ -1015,49 +1101,49 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="D28" s="10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>14</v>
@@ -1066,12 +1152,12 @@
         <v>40</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>22</v>
@@ -1080,12 +1166,12 @@
         <v>40</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>25</v>
@@ -1094,12 +1180,12 @@
         <v>40</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>20</v>
@@ -1108,7 +1194,165 @@
         <v>40</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="12"/>
+      <c r="D35" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="12"/>
+      <c r="D36" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="12"/>
+      <c r="D37" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="12"/>
+      <c r="D39" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="D40" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="12"/>
+      <c r="D41" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="12"/>
+      <c r="D42" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
include latest tagging file and update evidence map
</commit_message>
<xml_diff>
--- a/raw-data/RSV_attribute_hierarchy_Dec.xlsx
+++ b/raw-data/RSV_attribute_hierarchy_Dec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/z2211982/github/RSVcorrelates/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A23468B-9509-A346-8D83-D564AFB30B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7137FAAD-7EF0-8C4B-89CF-6C5D985E52C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5520" yWindow="1340" windowWidth="39280" windowHeight="20860" xr2:uid="{E5577812-52DB-7549-9224-56C8E4FDF043}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="88">
   <si>
     <t>level_1_attribute</t>
   </si>
@@ -291,6 +291,18 @@
   </si>
   <si>
     <t>older_adults</t>
+  </si>
+  <si>
+    <t>Outcome Reported</t>
+  </si>
+  <si>
+    <t>active_immunogenicity</t>
+  </si>
+  <si>
+    <t>passive_immunogenicity</t>
+  </si>
+  <si>
+    <t>efficacy</t>
   </si>
 </sst>
 </file>
@@ -312,7 +324,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -355,6 +367,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -368,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -410,6 +428,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -744,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B74C7C1-39D6-4543-AF62-37F03D7DCD25}">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1355,6 +1377,42 @@
         <v>83</v>
       </c>
     </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{1B74C7C1-39D6-4543-AF62-37F03D7DCD25}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>